<commit_message>
Images, more information added
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166926D9-9D7C-4BEF-8688-962A5F10EEE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CB3E33-202C-4FB0-B0F4-6287DAB41CBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="600" windowWidth="12920" windowHeight="9140" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Title</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Genre</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Seasons</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Mystery, Adventure, Comedy</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Disney Channel, Disney XD</t>
   </si>
   <si>
@@ -156,16 +150,78 @@
   </si>
   <si>
     <t>Lincoln Loud is an eleven-year-old boy who lives with ten sisters. With the help of his right-hand man Clyde, Lincoln finds new ways to survive in such a large family every day.</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Wander Over Yonder</t>
+  </si>
+  <si>
+    <t>Over the Garden Wall</t>
+  </si>
+  <si>
+    <t>Craig McCracken</t>
+  </si>
+  <si>
+    <t>Comedy, Adventure, Science Fantasy</t>
+  </si>
+  <si>
+    <t>Wander is is eager to help anyone in the galaxy, together with his friend Sylvia. Wander's friendliness often angers Lord Hater, who is bent on galactic domination, and his army of Watchdogs.</t>
+  </si>
+  <si>
+    <t>Two brothers find themselves lost in a mysterious land and try to find their way home.</t>
+  </si>
+  <si>
+    <t>Patrick McHale</t>
+  </si>
+  <si>
+    <t>Dark Fantasy</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNTA0Y2FiNjYtMmI3ZC00YTA2LWJkZTEtNDExZDgxZGM2OTc1XkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_CR0,0,683,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BYjQwZDhhNzctNTZjYy00NjYzLWE3ZjctNGQwZWY2Zjg5NTgwL2ltYWdlL2ltYWdlXkEyXkFqcGdeQXVyNTAyODkwOQ@@._V1_SY1000_CR0,0,701,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMTEzNDc3MDQ2NzNeQTJeQWpwZ15BbWU4MDYzMzUwMDIx._V1_SY1000_CR0,0,641,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNTk2NzEyNTQtZTQ5MS00MjAyLTgzMDMtNDNkYTBkM2M2OTU3XkEyXkFqcGdeQXVyODUwNjEzMzg@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNTNjMTM1YWYtZWQ3Yy00OGI1LWEyZjUtYTk3OTk5NGIxMzIyXkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_CR0,0,651,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BODBkZWI3MmItMWU2ZC00M2FhLTk1YWQtNjU5YzI0NzI0NmIxXkEyXkFqcGdeQXVyNzA0MTM4NjM@._V1_SY1000_CR0,0,681,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMGU5MWQ3ZWItMzEzMy00NjljLWFjYzUtMGMxNTk2YWEwMzMyXkEyXkFqcGdeQXVyNjExODE1MDc@._V1_SY1000_CR0,0,706,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BODMyNGMxZGEtY2RiZS00YTViLWIzYTctMmFhZDNmZTIyMTczXkEyXkFqcGdeQXVyOTk3NjY3NTM@._V1_SY1000_CR0,0,684,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNzJiM2JhZGYtODFkZC00ZjE5LWE2ZmItMmE0Y2JiMWFkMWFkXkEyXkFqcGdeQXVyODk4Nzg5NjE@._V1_SY1000_CR0,0,666,1000_AL_.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,13 +244,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,8 +577,8 @@
     <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6328125" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -534,241 +593,313 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>2012</v>
+      </c>
+      <c r="E2">
+        <v>2016</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>40</v>
-      </c>
-      <c r="H2">
-        <v>2012</v>
-      </c>
-      <c r="I2">
-        <v>2016</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3">
+        <v>1999</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>247</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
-      </c>
-      <c r="G3">
-        <v>247</v>
-      </c>
-      <c r="H3">
-        <v>1999</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>2013</v>
+      </c>
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>160</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>160</v>
-      </c>
-      <c r="H4">
-        <v>2013</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5">
+        <v>2015</v>
+      </c>
+      <c r="E5">
+        <v>2019</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>77</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>77</v>
-      </c>
-      <c r="H5">
-        <v>2015</v>
-      </c>
-      <c r="I5">
-        <v>2019</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6">
+        <v>2004</v>
+      </c>
+      <c r="E6">
+        <v>2007</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>53</v>
       </c>
-      <c r="H6">
-        <v>2004</v>
-      </c>
-      <c r="I6">
-        <v>2007</v>
+      <c r="I6" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>2019</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="H7">
-        <v>2019</v>
+      <c r="I7" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8">
+        <v>2016</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>164</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>164</v>
-      </c>
-      <c r="H8">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>2013</v>
+      </c>
+      <c r="E9">
         <v>2016</v>
       </c>
-      <c r="J8" t="s">
-        <v>19</v>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>2014</v>
+      </c>
+      <c r="E10">
+        <v>2014</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{C687F440-15DE-4058-9DA8-DDAF5748B96E}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{741E3E25-D8AD-4426-87AE-E238E9247835}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{AD7D1D3F-79F2-4FEA-97C8-126CFBF8E565}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New filters to find shows and networks
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CB3E33-202C-4FB0-B0F4-6287DAB41CBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D86DCDE-8B66-4CCC-80E4-074D906667C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
+    <workbookView xWindow="680" yWindow="510" windowWidth="12920" windowHeight="9140" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>Title</t>
   </si>
@@ -204,6 +204,45 @@
   </si>
   <si>
     <t>https://m.media-amazon.com/images/M/MV5BNzJiM2JhZGYtODFkZC00ZjE5LWE2ZmItMmE0Y2JiMWFkMWFkXkEyXkFqcGdeQXVyODk4Nzg5NjE@._V1_SY1000_CR0,0,666,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Foster's Home for Imaginary Friends</t>
+  </si>
+  <si>
+    <t>Rocko's Modern Life</t>
+  </si>
+  <si>
+    <t>Ducktales</t>
+  </si>
+  <si>
+    <t>Fantasy, Comedy, Adventure</t>
+  </si>
+  <si>
+    <t>A boy and his beloved imaginary friend are able to stay together at an orphanage of sorts for imaginary friends that children have outgrown to be adopted by new children.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNjYyNGFjOTctYzFmNC00NzdmLThhMDgtNjEzZTRmNzA3ODc5XkEyXkFqcGdeQXVyNjk1Njg5NTA@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Joe Murray</t>
+  </si>
+  <si>
+    <t>Satire, Slapstick</t>
+  </si>
+  <si>
+    <t>The wacky misadventures of an Australian wallaby and his friends as he finishes his transition to American life.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMjc5YmYwZmEtZjA3Ni00MWUxLWFjMmYtMzE3NTNiY2MyZTlmXkEyXkFqcGdeQXVyNjk1Njg5NTA@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>The comedy-adventure series chronicles the high-flying adventures of trillionaire Scrooge McDuck, his grandnephews - Huey, Dewey, and Louie - temperamental nephew Donald Duck, Launchpad McQuack, Mrs. Beakley, and her granddaughter Webby.</t>
+  </si>
+  <si>
+    <t>Matt Youngberg, Francisco Angones</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNTA2NTc5MzQwNV5BMl5BanBnXkFtZTgwOTY2ODI2MjI@._V1_SY1000_CR0,0,666,1000_AL_.jpg</t>
   </si>
 </sst>
 </file>
@@ -566,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,6 +929,99 @@
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>2004</v>
+      </c>
+      <c r="E11">
+        <v>2009</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>79</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>1993</v>
+      </c>
+      <c r="E12">
+        <v>1996</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>52</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13">
+        <v>2017</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>43</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
@@ -898,8 +1030,11 @@
     <hyperlink ref="I6" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
     <hyperlink ref="I7" r:id="rId5" xr:uid="{AD7D1D3F-79F2-4FEA-97C8-126CFBF8E565}"/>
     <hyperlink ref="I8" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
+    <hyperlink ref="I11" r:id="rId7" xr:uid="{468AE3DF-EF27-4866-8CD5-5A93DC948ED0}"/>
+    <hyperlink ref="I12" r:id="rId8" xr:uid="{EDC4BDC7-133C-467F-901E-836142661E00}"/>
+    <hyperlink ref="I13" r:id="rId9" xr:uid="{F71ADCC5-4CF9-4BFD-97D9-152126A218A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved filters, condensed filter.js
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D86DCDE-8B66-4CCC-80E4-074D906667C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A868710-DA29-47D4-AB86-EA99F82EFE3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="510" windowWidth="12920" windowHeight="9140" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>Title</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Intergalactic warrior Star Butterfly arrives on Earth to live with the Diaz family. She continues to battle villains throughout the universe and high school, mainly to protect her extremely powerful wand, an object that still confuses her.</t>
   </si>
   <si>
-    <t>Adventure, Magical Girl</t>
-  </si>
-  <si>
     <t>Disney XD</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>A boy and his beloved imaginary friend are able to stay together at an orphanage of sorts for imaginary friends that children have outgrown to be adopted by new children.</t>
   </si>
   <si>
-    <t>https://m.media-amazon.com/images/M/MV5BNjYyNGFjOTctYzFmNC00NzdmLThhMDgtNjEzZTRmNzA3ODc5XkEyXkFqcGdeQXVyNjk1Njg5NTA@._V1_.jpg</t>
-  </si>
-  <si>
     <t>Joe Murray</t>
   </si>
   <si>
@@ -243,13 +237,76 @@
   </si>
   <si>
     <t>https://m.media-amazon.com/images/M/MV5BNTA2NTc5MzQwNV5BMl5BanBnXkFtZTgwOTY2ODI2MjI@._V1_SY1000_CR0,0,666,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Adventure, Fantasy</t>
+  </si>
+  <si>
+    <t>Big Hero 6: The Series</t>
+  </si>
+  <si>
+    <t>Avatar: The Last Airbender</t>
+  </si>
+  <si>
+    <t>Craig of the Creek</t>
+  </si>
+  <si>
+    <t>Mark McCorkle, Bob Schooley, Nick Filippi</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>As the new prodigy at San Fransokyo Institute of Technology, Hiro now faces daunting academic challenges and the social trials of being the little man on campus. Off campus, the stakes are raised for the high-tech heroes as they must protect their city from an array of scientifically enhanced villains.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMjE5OTQyMDg3NV5BMl5BanBnXkFtZTgwNjMxODg5ODE@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Michael Dante DiMartino, Bryan Konietzko</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Fantasy</t>
+  </si>
+  <si>
+    <t>In a war-torn world of elemental magic, a young boy reawakens to undertake a dangerous mystic quest to fulfill his destiny as the Avatar, and bring peace to the world.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNzZlZmQyYTgtOWNmMy00NTNhLTgyOTYtNjhiOTllOGU2MDg5XkEyXkFqcGdeQXVyMjYxMzY2NDk@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Matt Burnett, Ben Levin</t>
+  </si>
+  <si>
+    <t>Craig of the Creek follows a young boy, Craig, and his two friends, Kelsey and JP, as they go on adventures within a world of untamed, kid-dominated wilderness in the creek.</t>
+  </si>
+  <si>
+    <t>Comedy, Adventure</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BYjRmZGRjNTYtM2M2Yi00OWM5LThiZmEtMjQ0Y2U1NGVmNWM1XkEyXkFqcGdeQXVyODQzMjA3OTQ@._V1_SY1000_CR0,0,721,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>The Fairly OddParents</t>
+  </si>
+  <si>
+    <t>After being tortured and humiliated by his babysitter, a ten year old boy is put under the care of two fairy godparents, who can grant him almost any wish, which leads to dire consequences.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BM2I0YjQ3NzgtMWE2Zi00NTgxLThlNDUtZTI0MjFlM2Y5NTM1XkEyXkFqcGdeQXVyNTUyMzE4Mzg@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Comedy, Fantasy</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/474x/00/8f/f0/008ff01ff11df6e5a84aac640946868f--imaginary-friends-cartoon-network.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +318,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -287,9 +352,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,51 +671,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6328125" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -679,7 +745,7 @@
         <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
@@ -687,121 +753,121 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D3">
-        <v>1999</v>
+        <v>2013</v>
+      </c>
+      <c r="E3">
+        <v>2016</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>43</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
         <v>12</v>
-      </c>
-      <c r="H3">
-        <v>247</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>2013</v>
+        <v>2015</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>160</v>
+        <v>77</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>2015</v>
-      </c>
-      <c r="E5">
-        <v>2019</v>
+        <v>1999</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>77</v>
+        <v>247</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>2004</v>
-      </c>
-      <c r="E6">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
@@ -809,28 +875,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D7">
-        <v>2019</v>
+        <v>2004</v>
+      </c>
+      <c r="E7">
+        <v>2009</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
         <v>22</v>
@@ -838,51 +907,48 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>2017</v>
+      </c>
+      <c r="F9" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>2013</v>
-      </c>
-      <c r="E9">
-        <v>2016</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -891,7 +957,7 @@
         <v>43</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
         <v>12</v>
@@ -899,31 +965,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>2014</v>
-      </c>
-      <c r="E10">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J10" t="s">
         <v>22</v>
@@ -931,31 +994,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D11">
-        <v>2004</v>
+        <v>2014</v>
       </c>
       <c r="E11">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
         <v>22</v>
@@ -963,31 +1026,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>1993</v>
+        <v>2004</v>
       </c>
       <c r="E12">
-        <v>1996</v>
+        <v>2007</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
@@ -995,46 +1058,174 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D13">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>70</v>
       </c>
-      <c r="J13" t="s">
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <v>2017</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>39</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15">
+        <v>2005</v>
+      </c>
+      <c r="E15">
+        <v>2008</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>61</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>1993</v>
+      </c>
+      <c r="E16">
+        <v>1996</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>52</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17">
+        <v>2001</v>
+      </c>
+      <c r="E17">
+        <v>2017</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>161</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{C687F440-15DE-4058-9DA8-DDAF5748B96E}"/>
-    <hyperlink ref="I5" r:id="rId3" xr:uid="{741E3E25-D8AD-4426-87AE-E238E9247835}"/>
-    <hyperlink ref="I6" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
-    <hyperlink ref="I7" r:id="rId5" xr:uid="{AD7D1D3F-79F2-4FEA-97C8-126CFBF8E565}"/>
-    <hyperlink ref="I8" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
-    <hyperlink ref="I11" r:id="rId7" xr:uid="{468AE3DF-EF27-4866-8CD5-5A93DC948ED0}"/>
-    <hyperlink ref="I12" r:id="rId8" xr:uid="{EDC4BDC7-133C-467F-901E-836142661E00}"/>
-    <hyperlink ref="I13" r:id="rId9" xr:uid="{F71ADCC5-4CF9-4BFD-97D9-152126A218A1}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
+    <hyperlink ref="I10" r:id="rId2" xr:uid="{C687F440-15DE-4058-9DA8-DDAF5748B96E}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{741E3E25-D8AD-4426-87AE-E238E9247835}"/>
+    <hyperlink ref="I12" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{AD7D1D3F-79F2-4FEA-97C8-126CFBF8E565}"/>
+    <hyperlink ref="I6" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
+    <hyperlink ref="I16" r:id="rId7" xr:uid="{EDC4BDC7-133C-467F-901E-836142661E00}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{F71ADCC5-4CF9-4BFD-97D9-152126A218A1}"/>
+    <hyperlink ref="I14" r:id="rId9" xr:uid="{C249B5CA-56F6-4E1F-8A0A-BCE3508EA7F0}"/>
+    <hyperlink ref="I15" r:id="rId10" xr:uid="{EF987F64-B534-42AE-A532-87C7BE597BD9}"/>
+    <hyperlink ref="I13" r:id="rId11" xr:uid="{21977A26-2445-42E4-BC2B-86C461D9165A}"/>
+    <hyperlink ref="I17" r:id="rId12" xr:uid="{EAB1EF2F-1F76-49CA-A1A4-9AF99C2A7E79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited styles, experimenting with button to watch trailers
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A868710-DA29-47D4-AB86-EA99F82EFE3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24FE39B-54DA-47E5-B965-BBCB0F1E0174}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Title</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>https://i.pinimg.com/474x/00/8f/f0/008ff01ff11df6e5a84aac640946868f--imaginary-friends-cartoon-network.jpg</t>
+  </si>
+  <si>
+    <t>Trailer</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yfUDIPUETUg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=izT6jYXZceA</t>
   </si>
 </sst>
 </file>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,9 +694,10 @@
     <col min="4" max="5" width="8.7265625" customWidth="1"/>
     <col min="6" max="6" width="31.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -718,8 +728,11 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -750,8 +763,11 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -782,8 +798,11 @@
       <c r="J3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -815,7 +834,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -844,7 +863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -873,7 +892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -905,7 +924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -934,7 +953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -963,7 +982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -992,7 +1011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1024,7 +1043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1085,7 +1104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -1146,7 +1165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1224,8 +1243,10 @@
     <hyperlink ref="I15" r:id="rId10" xr:uid="{EF987F64-B534-42AE-A532-87C7BE597BD9}"/>
     <hyperlink ref="I13" r:id="rId11" xr:uid="{21977A26-2445-42E4-BC2B-86C461D9165A}"/>
     <hyperlink ref="I17" r:id="rId12" xr:uid="{EAB1EF2F-1F76-49CA-A1A4-9AF99C2A7E79}"/>
+    <hyperlink ref="K2" r:id="rId13" xr:uid="{EE225C8B-9E4D-4243-BD17-CB23D3C05D45}"/>
+    <hyperlink ref="K3" r:id="rId14" xr:uid="{F5F0680B-4A4A-40DC-A351-344D616DFF58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored addition of HTML elements in JavaScript, removed unused filters
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24FE39B-54DA-47E5-B965-BBCB0F1E0174}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF07E7B7-17ED-4C28-BA04-D93ADE029853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
+    <workbookView xWindow="7070" yWindow="240" windowWidth="12130" windowHeight="9530" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
   <si>
     <t>Title</t>
   </si>
@@ -309,6 +309,90 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=izT6jYXZceA</t>
+  </si>
+  <si>
+    <t>Randy Cunningham: 9th Grade Ninja</t>
+  </si>
+  <si>
+    <t>Penn Zero: Part Time Hero</t>
+  </si>
+  <si>
+    <t>Milo Murphy's Law</t>
+  </si>
+  <si>
+    <t>The Adventures of Jimmy Neutron: Boy Genius</t>
+  </si>
+  <si>
+    <t>Camp Lazlo</t>
+  </si>
+  <si>
+    <t>Chowder</t>
+  </si>
+  <si>
+    <t>Jed Elinoff, Scott Thomas</t>
+  </si>
+  <si>
+    <t>Action, Comedy</t>
+  </si>
+  <si>
+    <t>An ordinary ninth grader is chosen to become The Ninja. He is tasked with protecting the town from evil as well as balancing his school life with friends and homework.</t>
+  </si>
+  <si>
+    <t>Jared Bush, Sam Levine</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Science Fantasy</t>
+  </si>
+  <si>
+    <t>Penn Zero is not your average kid - every day he's zapped into another dimension with his friends to save the world.</t>
+  </si>
+  <si>
+    <t>Dan Povenmire, Jeff "Swampy" Marsh</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMjQxMDY0NjY1MV5BMl5BanBnXkFtZTgwNzQwNDc4OTE@._V1_SY1000_SX690_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNTIzMzliOWItNDNhYi00N2YyLWI1NTQtMjMxMTc1ZjhlMDk4XkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_SX642_AL_.jpg</t>
+  </si>
+  <si>
+    <t>An animated comedy adventure series that follows 13-year-old Milo Murphy, the fictional great-great-great-great grandson of the Murphy's Law namesake.</t>
+  </si>
+  <si>
+    <t>John A. Davis, Keith Alcorn</t>
+  </si>
+  <si>
+    <t>Adventure, Science Fiction</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMWRlNTRkM2ItNDkwMC00ZjNmLWI2ZDQtNWI0MTllMGU5OTVjXkEyXkFqcGdeQXVyNTUyMzE4Mzg@._V1_SY1000_CR0,0,750,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>A young boy, who happens to be a genius, lives in a small town with his family and friends and often gets into crazy adventures with them involving the things he invents.</t>
+  </si>
+  <si>
+    <t>Comedy, Slapstick</t>
+  </si>
+  <si>
+    <t>Bean Scout Lazlo, a fun-loving, free-spirited monkey, and his two bunkmates Raj and Clam, wreak havoc on a very structured summer camp.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNDQwYzI3YzQtZTQyMy00OTY3LWEyMmMtNTExZTQzNmY0OTdiL2ltYWdlXkEyXkFqcGdeQXVyNjQwOTYyNTY@._V1_SY1000_SX750_AL_.jpg</t>
+  </si>
+  <si>
+    <t>C. H. Greenblatt</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BYmFlMDZkMWItZjVkMi00MzhmLWFhMjUtYTRjNjE1ZjE5ZGMzXkEyXkFqcGdeQXVyNTAyODkwOQ@@._V1_SY1000_CR0,0,666,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>In Marzipan City, the young, excitable food-loving Chowder is the apprentice of Mung Daal, a very old chef who runs a catering company with his wife, Truffles and assistant, Shnitzel.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BN2VmMDgyODAtYWI3Ni00NWZiLTkxODktZTJlYTc0MjA1M2UxXkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_CR0,0,703,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
 </sst>
 </file>
@@ -361,10 +445,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -680,18 +770,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6328125" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="3" customWidth="1"/>
     <col min="6" max="6" width="31.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="43.6328125" bestFit="1" customWidth="1"/>
@@ -710,7 +801,7 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -745,7 +836,7 @@
       <c r="D2">
         <v>2012</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>2016</v>
       </c>
       <c r="F2" t="s">
@@ -780,7 +871,7 @@
       <c r="D3">
         <v>2013</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>2016</v>
       </c>
       <c r="F3" t="s">
@@ -815,7 +906,7 @@
       <c r="D4">
         <v>2015</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>2019</v>
       </c>
       <c r="F4" t="s">
@@ -847,6 +938,9 @@
       <c r="D5">
         <v>1999</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
@@ -876,6 +970,9 @@
       <c r="D6">
         <v>2016</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
@@ -905,7 +1002,7 @@
       <c r="D7">
         <v>2004</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>2009</v>
       </c>
       <c r="F7" t="s">
@@ -937,6 +1034,9 @@
       <c r="D8">
         <v>2019</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
@@ -966,6 +1066,9 @@
       <c r="D9">
         <v>2017</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F9" t="s">
         <v>43</v>
       </c>
@@ -995,6 +1098,9 @@
       <c r="D10">
         <v>2013</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F10" t="s">
         <v>21</v>
       </c>
@@ -1024,7 +1130,7 @@
       <c r="D11">
         <v>2014</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>2014</v>
       </c>
       <c r="F11" t="s">
@@ -1056,7 +1162,7 @@
       <c r="D12">
         <v>2004</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>2007</v>
       </c>
       <c r="F12" t="s">
@@ -1088,6 +1194,9 @@
       <c r="D13">
         <v>2018</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F13" t="s">
         <v>83</v>
       </c>
@@ -1117,6 +1226,9 @@
       <c r="D14">
         <v>2017</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F14" t="s">
         <v>74</v>
       </c>
@@ -1146,7 +1258,7 @@
       <c r="D15">
         <v>2005</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>2008</v>
       </c>
       <c r="F15" t="s">
@@ -1178,7 +1290,7 @@
       <c r="D16">
         <v>1993</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>1996</v>
       </c>
       <c r="F16" t="s">
@@ -1210,7 +1322,7 @@
       <c r="D17">
         <v>2001</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>2017</v>
       </c>
       <c r="F17" t="s">
@@ -1227,6 +1339,198 @@
       </c>
       <c r="J17" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>2012</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19">
+        <v>2014</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2017</v>
+      </c>
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>61</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20">
+        <v>2016</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21">
+        <v>2002</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2006</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>81</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22">
+        <v>2005</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2008</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>120</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23">
+        <v>2007</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2010</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>93</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1245,8 +1549,11 @@
     <hyperlink ref="I17" r:id="rId12" xr:uid="{EAB1EF2F-1F76-49CA-A1A4-9AF99C2A7E79}"/>
     <hyperlink ref="K2" r:id="rId13" xr:uid="{EE225C8B-9E4D-4243-BD17-CB23D3C05D45}"/>
     <hyperlink ref="K3" r:id="rId14" xr:uid="{F5F0680B-4A4A-40DC-A351-344D616DFF58}"/>
+    <hyperlink ref="I21" r:id="rId15" xr:uid="{9D32754F-CBDD-4ABD-A58F-6CBB215DE1BD}"/>
+    <hyperlink ref="I22" r:id="rId16" xr:uid="{300A07A2-D057-480A-9245-1A15BF787E5E}"/>
+    <hyperlink ref="I23" r:id="rId17" xr:uid="{3D1EE69D-01E8-41A7-9DA4-76719B184162}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
May 2023 cartoon update
</commit_message>
<xml_diff>
--- a/cartoons.xlsx
+++ b/cartoons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\Cartoon Chronology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4386c1414a532859/Documents/Cartoons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF07E7B7-17ED-4C28-BA04-D93ADE029853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{EF07E7B7-17ED-4C28-BA04-D93ADE029853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B36DA2B-2BD1-4430-8545-B7B79A5B43FC}"/>
   <bookViews>
-    <workbookView xWindow="7070" yWindow="240" windowWidth="12130" windowHeight="9530" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8A3ABA9-09A2-4729-B2D4-CF6085F5D583}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="158">
   <si>
     <t>Title</t>
   </si>
@@ -179,18 +179,12 @@
     <t>https://m.media-amazon.com/images/M/MV5BNTA0Y2FiNjYtMmI3ZC00YTA2LWJkZTEtNDExZDgxZGM2OTc1XkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_CR0,0,683,1000_AL_.jpg</t>
   </si>
   <si>
-    <t>https://m.media-amazon.com/images/M/MV5BYjQwZDhhNzctNTZjYy00NjYzLWE3ZjctNGQwZWY2Zjg5NTgwL2ltYWdlL2ltYWdlXkEyXkFqcGdeQXVyNTAyODkwOQ@@._V1_SY1000_CR0,0,701,1000_AL_.jpg</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/M/MV5BMTEzNDc3MDQ2NzNeQTJeQWpwZ15BbWU4MDYzMzUwMDIx._V1_SY1000_CR0,0,641,1000_AL_.jpg</t>
   </si>
   <si>
     <t>https://m.media-amazon.com/images/M/MV5BNTk2NzEyNTQtZTQ5MS00MjAyLTgzMDMtNDNkYTBkM2M2OTU3XkEyXkFqcGdeQXVyODUwNjEzMzg@._V1_.jpg</t>
   </si>
   <si>
-    <t>https://m.media-amazon.com/images/M/MV5BNTNjMTM1YWYtZWQ3Yy00OGI1LWEyZjUtYTk3OTk5NGIxMzIyXkEyXkFqcGdeQXVyMzM4NjcxOTc@._V1_SY1000_CR0,0,651,1000_AL_.jpg</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/M/MV5BODBkZWI3MmItMWU2ZC00M2FhLTk1YWQtNjU5YzI0NzI0NmIxXkEyXkFqcGdeQXVyNzA0MTM4NjM@._V1_SY1000_CR0,0,681,1000_AL_.jpg</t>
   </si>
   <si>
@@ -393,6 +387,123 @@
   </si>
   <si>
     <t>Present</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNWQ1YWI0YjgtNWNmYy00NTY0LWJjZjgtMGFmMDU1OGM5Y2FiXkEyXkFqcGdeQXVyMTA3MzQ4MTg0._V1_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BYzhjNzI0NWEtMzEyYy00OGViLThhMjctMWQxNGQ3Y2IzOTY4XkEyXkFqcGdeQXVyNjAwNDUxODI@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Amphibia</t>
+  </si>
+  <si>
+    <t>The Owl House</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Inside Job</t>
+  </si>
+  <si>
+    <t>The Ghost and Molly McGee</t>
+  </si>
+  <si>
+    <t>Big City Greens</t>
+  </si>
+  <si>
+    <t>Kiff</t>
+  </si>
+  <si>
+    <t>Marvel's Moon Girl and Devil Dinosaur</t>
+  </si>
+  <si>
+    <t>Matt Braly</t>
+  </si>
+  <si>
+    <t>Dana Terrace</t>
+  </si>
+  <si>
+    <t>The Houghton Brothers</t>
+  </si>
+  <si>
+    <t>Lucy Heavens, Nic Smal</t>
+  </si>
+  <si>
+    <t>Disney Channel</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Ordinary Anne Boonchuy, 13, finds a music box that sends her to Amphibia, a world full of frogs, toads, and giant insects. With help from Sprig, she must adjust to life in Amphibia and discover the first true friendship in her life.</t>
+  </si>
+  <si>
+    <t>Action, Adventure</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BN2U1YTg4ZjUtMzMyMS00N2ZiLTg3ODMtOTAwZmU2YmMxYjFjXkEyXkFqcGdeQXVyMTkxNjUyNQ@@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BOGQ0MDQyYWMtNjdlYy00ZDAyLWE5YTItMzcyMjllZTA4MTcyXkEyXkFqcGdeQXVyMjEzNTg5Mzk@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Accidentally sent to the world of the Boiling Isles before a trip to summer camp, a teenage human named Luz longs to become a witch and is aided by rebellious Eda and pint-sized demon King.</t>
+  </si>
+  <si>
+    <t>A fearless blue-haired girl named Hilda leaves the forest to go to town and find new friends, great adventures, magic and mysterious creatures who might be dangerous.</t>
+  </si>
+  <si>
+    <t>Kurt Mueller, Luke Pearson, Stephanie Simpson</t>
+  </si>
+  <si>
+    <t>Adventure, Comedy</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNGQ0NWNhODUtNTI4MC00NTcxLWE4ZmQtZGY0NGU0NDIwNGQxXkEyXkFqcGdeQXVyMTMxODk2OTU@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Shion Takeuchi</t>
+  </si>
+  <si>
+    <t>For employees of the Deep State, conspiracies aren't just theories, they're fact. And keeping them a secret is a full-time job.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BZTg5YjE1YzktYjRmZC00Y2VjLThiMDItOTcwODRhMjRjZDQ1XkEyXkFqcGdeQXVyMTEzMTI1Mjk3._V1_.jpg</t>
+  </si>
+  <si>
+    <t>A grumpy ghost named Scratch is eternally cursed to be in the presence of polar opposite Molly McGee, a cheerful tween.</t>
+  </si>
+  <si>
+    <t>Bill Motz, Bob Roth</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BMDJiZWMwY2MtODZhMC00Nzg1LWI0Y2EtYzJlYTEwZGYwYTk4XkEyXkFqcGdeQXVyMTE2NDA4MDMy._V1_.jpg</t>
+  </si>
+  <si>
+    <t>The adventurous life of Cricket Green, a country boy who moves with his family from their rural farm to a modern metropolis.</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BNzA4ODUwNDA0OF5BMl5BanBnXkFtZTgwMjc1NjM1NTM@._V1_.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://m.media-amazon.com/images/M/MV5BMDA4ZDIwMTUtZWUyYS00YWY3LWJjODgtNWIwYjcxNGUxMzE0XkEyXkFqcGdeQXVyMTEzMTI1Mjk3._V1_.jpg </t>
+  </si>
+  <si>
+    <t>After 13-year-old super-genius Lunella accidentally brings ten-ton T-Rex, Devil Dinosaur into present-day New York City via a time vortex, the duo works together to protect the city's Lower East Side from danger.</t>
+  </si>
+  <si>
+    <t>Jeffrey M. Howard, Kate Kondell, Steve Loter</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Superhero</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BY2QwYmZmYWMtY2VhZi00ZGFiLTg0N2UtNDg4OTNjYzA0MWQ0XkEyXkFqcGdeQXVyODk4OTc3MTY@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>Follow the adventures of best friends Kiff, an optimistic squirrel, and Barry, a mellow bunny, as they take Table Town by storm with their endless adventures.</t>
   </si>
 </sst>
 </file>
@@ -471,6 +582,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,25 +885,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C551C43F-ED77-4413-9AF9-4A44107BED3A}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6328125" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -820,10 +935,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -849,16 +964,16 @@
         <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -890,114 +1005,114 @@
         <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2022</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>106</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5">
+        <v>2020</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
         <v>26</v>
       </c>
-      <c r="D4">
-        <v>2015</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>77</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>1999</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>247</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6">
-        <v>2016</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>164</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7">
         <v>2004</v>
@@ -1006,7 +1121,7 @@
         <v>2009</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -1015,13 +1130,13 @@
         <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1034,450 +1149,450 @@
       <c r="D8">
         <v>2019</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>120</v>
+      <c r="E8" s="3">
+        <v>2021</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="D9">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>2013</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2014</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>160</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>2014</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2014</v>
+        <v>2018</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="J11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12">
-        <v>2004</v>
+        <v>2015</v>
       </c>
       <c r="E12" s="3">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D13">
-        <v>2018</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>120</v>
+        <v>2016</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2019</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>2017</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>120</v>
+        <v>2004</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2007</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>2005</v>
-      </c>
-      <c r="E15" s="3">
-        <v>2008</v>
+        <v>1999</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H15">
-        <v>61</v>
+        <v>284</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D16">
-        <v>1993</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1996</v>
+        <v>2016</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H16">
-        <v>52</v>
+        <v>241</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D17">
-        <v>2001</v>
+        <v>2017</v>
       </c>
       <c r="E17" s="3">
+        <v>2021</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>2013</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>160</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19">
         <v>2017</v>
       </c>
-      <c r="F17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17">
-        <v>161</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18">
-        <v>2012</v>
-      </c>
-      <c r="E18" s="3">
-        <v>2015</v>
-      </c>
-      <c r="F18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>100</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19">
-        <v>2014</v>
-      </c>
       <c r="E19" s="3">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="J19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="D20">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21">
+        <v>2023</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>16</v>
       </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>40</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21">
-        <v>2002</v>
-      </c>
-      <c r="E21" s="3">
-        <v>2006</v>
-      </c>
-      <c r="F21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>81</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>2005</v>
@@ -1486,74 +1601,339 @@
         <v>2008</v>
       </c>
       <c r="F22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>61</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23">
+        <v>1993</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1996</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>52</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24">
+        <v>2018</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>80</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25">
+        <v>2001</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2017</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>161</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26">
+        <v>2012</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27">
+        <v>2014</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2017</v>
+      </c>
+      <c r="F27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>61</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28">
+        <v>2021</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2022</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29">
+        <v>2002</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2006</v>
+      </c>
+      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>81</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30">
+        <v>2005</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2008</v>
+      </c>
+      <c r="F30" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>120</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="H22">
-        <v>120</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31">
+        <v>2007</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2010</v>
+      </c>
+      <c r="F31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>93</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23">
-        <v>2007</v>
-      </c>
-      <c r="E23" s="3">
-        <v>2010</v>
-      </c>
-      <c r="F23" t="s">
-        <v>113</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
-      <c r="H23">
-        <v>93</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="J31" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
-    <hyperlink ref="I10" r:id="rId2" xr:uid="{C687F440-15DE-4058-9DA8-DDAF5748B96E}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{741E3E25-D8AD-4426-87AE-E238E9247835}"/>
-    <hyperlink ref="I12" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
+    <hyperlink ref="I15" r:id="rId1" xr:uid="{7C1FFC32-9DDA-4862-B745-E10D7BEE8ADF}"/>
+    <hyperlink ref="I18" r:id="rId2" xr:uid="{C687F440-15DE-4058-9DA8-DDAF5748B96E}"/>
+    <hyperlink ref="I12" r:id="rId3" xr:uid="{741E3E25-D8AD-4426-87AE-E238E9247835}"/>
+    <hyperlink ref="I14" r:id="rId4" xr:uid="{537F35B5-F5CC-4A50-8C74-35081A0677BF}"/>
     <hyperlink ref="I8" r:id="rId5" xr:uid="{AD7D1D3F-79F2-4FEA-97C8-126CFBF8E565}"/>
-    <hyperlink ref="I6" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
-    <hyperlink ref="I16" r:id="rId7" xr:uid="{EDC4BDC7-133C-467F-901E-836142661E00}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{F71ADCC5-4CF9-4BFD-97D9-152126A218A1}"/>
-    <hyperlink ref="I14" r:id="rId9" xr:uid="{C249B5CA-56F6-4E1F-8A0A-BCE3508EA7F0}"/>
-    <hyperlink ref="I15" r:id="rId10" xr:uid="{EF987F64-B534-42AE-A532-87C7BE597BD9}"/>
-    <hyperlink ref="I13" r:id="rId11" xr:uid="{21977A26-2445-42E4-BC2B-86C461D9165A}"/>
-    <hyperlink ref="I17" r:id="rId12" xr:uid="{EAB1EF2F-1F76-49CA-A1A4-9AF99C2A7E79}"/>
+    <hyperlink ref="I16" r:id="rId6" xr:uid="{399CE115-1BB9-462B-AD32-6BA733BD5C79}"/>
+    <hyperlink ref="I23" r:id="rId7" xr:uid="{EDC4BDC7-133C-467F-901E-836142661E00}"/>
+    <hyperlink ref="I17" r:id="rId8" xr:uid="{F71ADCC5-4CF9-4BFD-97D9-152126A218A1}"/>
+    <hyperlink ref="I19" r:id="rId9" xr:uid="{C249B5CA-56F6-4E1F-8A0A-BCE3508EA7F0}"/>
+    <hyperlink ref="I22" r:id="rId10" xr:uid="{EF987F64-B534-42AE-A532-87C7BE597BD9}"/>
+    <hyperlink ref="I11" r:id="rId11" xr:uid="{21977A26-2445-42E4-BC2B-86C461D9165A}"/>
+    <hyperlink ref="I25" r:id="rId12" xr:uid="{EAB1EF2F-1F76-49CA-A1A4-9AF99C2A7E79}"/>
     <hyperlink ref="K2" r:id="rId13" xr:uid="{EE225C8B-9E4D-4243-BD17-CB23D3C05D45}"/>
     <hyperlink ref="K3" r:id="rId14" xr:uid="{F5F0680B-4A4A-40DC-A351-344D616DFF58}"/>
-    <hyperlink ref="I21" r:id="rId15" xr:uid="{9D32754F-CBDD-4ABD-A58F-6CBB215DE1BD}"/>
-    <hyperlink ref="I22" r:id="rId16" xr:uid="{300A07A2-D057-480A-9245-1A15BF787E5E}"/>
-    <hyperlink ref="I23" r:id="rId17" xr:uid="{3D1EE69D-01E8-41A7-9DA4-76719B184162}"/>
+    <hyperlink ref="I29" r:id="rId15" xr:uid="{9D32754F-CBDD-4ABD-A58F-6CBB215DE1BD}"/>
+    <hyperlink ref="I30" r:id="rId16" xr:uid="{300A07A2-D057-480A-9245-1A15BF787E5E}"/>
+    <hyperlink ref="I31" r:id="rId17" xr:uid="{3D1EE69D-01E8-41A7-9DA4-76719B184162}"/>
+    <hyperlink ref="I10" r:id="rId18" xr:uid="{2D102C2A-B995-4733-BD11-AEA77A25C427}"/>
+    <hyperlink ref="I4" r:id="rId19" xr:uid="{0D62B083-972C-40AF-BE09-71169F573881}"/>
+    <hyperlink ref="I5" r:id="rId20" xr:uid="{398D8762-495F-4D6D-A768-56A7D5579996}"/>
+    <hyperlink ref="I6" r:id="rId21" xr:uid="{B57C187B-7287-4D64-9E5C-626EE3E8CFB2}"/>
+    <hyperlink ref="I28" r:id="rId22" xr:uid="{10BB1F6C-B81C-4246-BE8C-3569E02394D6}"/>
+    <hyperlink ref="I9" r:id="rId23" xr:uid="{C36B0F0B-9E11-4AB9-A36C-A6A8B501D39A}"/>
+    <hyperlink ref="I24" r:id="rId24" xr:uid="{9594B400-3F0C-425B-BDF9-918B56E17F03}"/>
+    <hyperlink ref="I20" r:id="rId25" xr:uid="{CF294E67-08F8-403A-808A-90A2BE4B7E2B}"/>
+    <hyperlink ref="I21" r:id="rId26" xr:uid="{B1B9994E-7FEB-4DA3-BF37-C138EC8F910D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>